<commit_message>
Tugas reang mah ws selesai
</commit_message>
<xml_diff>
--- a/rata-rata_curr-ch.xlsx
+++ b/rata-rata_curr-ch.xlsx
@@ -1,27 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hakim\Desktop\New folder\rata-rata_yuh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C186F96-829E-482C-A199-EC5F8853AF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DAC38E-788F-4F46-8309-DF0250E91817}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7875" xr2:uid="{71251406-F57A-4761-B60D-ABCE191B0F07}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{71251406-F57A-4761-B60D-ABCE191B0F07}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames>
+    <definedName name="_8080" localSheetId="0">Sheet1!$G$2:$G$101</definedName>
+  </definedNames>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{5ECAB623-B99E-4049-AA0A-C508090BAC5B}" name="Connection" type="4" refreshedVersion="6" background="1" saveData="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://csv.test:8080" htmlFormat="all"/>
+  </connection>
+</connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -52,10 +69,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -81,8 +105,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -98,6 +128,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="8080" preserveFormatting="0" connectionId="1" xr16:uid="{8A364F30-C260-4E37-8E09-53416E6DC970}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -399,11 +433,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00408168-C694-4F30-8EA3-B92B936D369B}">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -438,6 +476,15 @@
       <c r="C2">
         <v>59.376069999999999</v>
       </c>
+      <c r="E2">
+        <v>112.666666666666</v>
+      </c>
+      <c r="F2" s="1">
+        <v>67871.213675213599</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1582.05982905982</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -449,6 +496,15 @@
       <c r="C3">
         <v>44.26896</v>
       </c>
+      <c r="E3">
+        <v>88.397899649941607</v>
+      </c>
+      <c r="F3" s="1">
+        <v>53340.894399066499</v>
+      </c>
+      <c r="G3" s="2">
+        <v>404.75845974329002</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -460,6 +516,15 @@
       <c r="C4">
         <v>65.642110000000002</v>
       </c>
+      <c r="E4">
+        <v>85.842105263157805</v>
+      </c>
+      <c r="F4" s="1">
+        <v>51816.673684210502</v>
+      </c>
+      <c r="G4" s="2">
+        <v>832.36842105263099</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -471,6 +536,15 @@
       <c r="C5">
         <v>1.5</v>
       </c>
+      <c r="E5">
+        <v>131</v>
+      </c>
+      <c r="F5" s="1">
+        <v>78741.5</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1164.5</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -482,6 +556,15 @@
       <c r="C6">
         <v>67.092060000000004</v>
       </c>
+      <c r="E6">
+        <v>90.914285714285697</v>
+      </c>
+      <c r="F6" s="1">
+        <v>54868.1095238095</v>
+      </c>
+      <c r="G6" s="2">
+        <v>744.41904761904698</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -493,6 +576,15 @@
       <c r="C7">
         <v>17.530609999999999</v>
       </c>
+      <c r="E7">
+        <v>106.714285714285</v>
+      </c>
+      <c r="F7" s="1">
+        <v>64262.959183673403</v>
+      </c>
+      <c r="G7" s="2">
+        <v>4590.3877551020396</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -504,6 +596,15 @@
       <c r="C8">
         <v>63.259569999999997</v>
       </c>
+      <c r="E8">
+        <v>85.493617021276506</v>
+      </c>
+      <c r="F8" s="1">
+        <v>51585.431205673704</v>
+      </c>
+      <c r="G8" s="2">
+        <v>708.143262411347</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -515,6 +616,15 @@
       <c r="C9">
         <v>79.165139999999994</v>
       </c>
+      <c r="E9">
+        <v>85.682568807339393</v>
+      </c>
+      <c r="F9" s="1">
+        <v>51703.163302752197</v>
+      </c>
+      <c r="G9" s="2">
+        <v>516.34862385321105</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -526,6 +636,15 @@
       <c r="C10">
         <v>98.196830000000006</v>
       </c>
+      <c r="E10">
+        <v>92.219457013574598</v>
+      </c>
+      <c r="F10" s="1">
+        <v>55624.187782805398</v>
+      </c>
+      <c r="G10" s="2">
+        <v>671.08144796379997</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -537,6 +656,15 @@
       <c r="C11">
         <v>66.347830000000002</v>
       </c>
+      <c r="E11">
+        <v>69.608695652173907</v>
+      </c>
+      <c r="F11" s="1">
+        <v>42036.391304347802</v>
+      </c>
+      <c r="G11" s="2">
+        <v>578.13043478260795</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -548,6 +676,15 @@
       <c r="C12">
         <v>55.125</v>
       </c>
+      <c r="E12">
+        <v>109.47159090909</v>
+      </c>
+      <c r="F12" s="1">
+        <v>65965.909090909001</v>
+      </c>
+      <c r="G12" s="2">
+        <v>387.10795454545399</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -559,6 +696,15 @@
       <c r="C13">
         <v>29.21875</v>
       </c>
+      <c r="E13">
+        <v>110.90625</v>
+      </c>
+      <c r="F13" s="1">
+        <v>66820.25</v>
+      </c>
+      <c r="G13" s="2">
+        <v>2874.703125</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -570,6 +716,15 @@
       <c r="C14">
         <v>47.68947</v>
       </c>
+      <c r="E14">
+        <v>89.513157894736807</v>
+      </c>
+      <c r="F14" s="1">
+        <v>54013.310526315698</v>
+      </c>
+      <c r="G14" s="2">
+        <v>503.56052631578899</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -581,6 +736,15 @@
       <c r="C15">
         <v>11.426830000000001</v>
       </c>
+      <c r="E15">
+        <v>116.012195121951</v>
+      </c>
+      <c r="F15" s="1">
+        <v>69915.195121951198</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1321.7439024390201</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -592,8 +756,17 @@
       <c r="C16">
         <v>83.309520000000006</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>105.312925170068</v>
+      </c>
+      <c r="F16" s="1">
+        <v>63442.346938775503</v>
+      </c>
+      <c r="G16" s="2">
+        <v>241.55782312925101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -603,8 +776,17 @@
       <c r="C17">
         <v>15.72</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>117.48</v>
+      </c>
+      <c r="F17" s="1">
+        <v>70785.16</v>
+      </c>
+      <c r="G17" s="2">
+        <v>101.32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -614,8 +796,17 @@
       <c r="C18">
         <v>49.575760000000002</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>96.219696969696898</v>
+      </c>
+      <c r="F18" s="1">
+        <v>57989.825757575702</v>
+      </c>
+      <c r="G18" s="2">
+        <v>775.62121212121201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -625,8 +816,17 @@
       <c r="C19">
         <v>31.69136</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>84.740740740740705</v>
+      </c>
+      <c r="F19" s="1">
+        <v>51131.777777777701</v>
+      </c>
+      <c r="G19" s="2">
+        <v>2141.54320987654</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -636,8 +836,17 @@
       <c r="C20">
         <v>42.696129999999997</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>111.88950276243</v>
+      </c>
+      <c r="F20" s="1">
+        <v>67417.596685082797</v>
+      </c>
+      <c r="G20" s="2">
+        <v>388.53591160220901</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -647,8 +856,17 @@
       <c r="C21">
         <v>61.076920000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>109.923076923076</v>
+      </c>
+      <c r="F21" s="1">
+        <v>66259.076923076893</v>
+      </c>
+      <c r="G21" s="2">
+        <v>661.47252747252696</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -658,8 +876,17 @@
       <c r="C22">
         <v>20.4953</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>91.278996865203695</v>
+      </c>
+      <c r="F22" s="1">
+        <v>55085.905956112802</v>
+      </c>
+      <c r="G22" s="2">
+        <v>1233.5768025078301</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -669,8 +896,17 @@
       <c r="C23">
         <v>26.696159999999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>81.908629441624299</v>
+      </c>
+      <c r="F23" s="1">
+        <v>49450.907179115296</v>
+      </c>
+      <c r="G23" s="2">
+        <v>833.30021754894801</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -680,8 +916,17 @@
       <c r="C24">
         <v>32.538460000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>59</v>
+      </c>
+      <c r="F24" s="1">
+        <v>35632.512820512798</v>
+      </c>
+      <c r="G24" s="2">
+        <v>492.94871794871699</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -691,8 +936,17 @@
       <c r="C25">
         <v>52.091500000000003</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>92.074074074074005</v>
+      </c>
+      <c r="F25" s="1">
+        <v>55568.265795206898</v>
+      </c>
+      <c r="G25" s="2">
+        <v>511.228758169934</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -702,8 +956,17 @@
       <c r="C26">
         <v>71.654790000000006</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>98.241095890410904</v>
+      </c>
+      <c r="F26" s="1">
+        <v>59268.030136986301</v>
+      </c>
+      <c r="G26" s="2">
+        <v>556.841095890411</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -713,8 +976,17 @@
       <c r="C27">
         <v>54.693390000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>88.490981963927794</v>
+      </c>
+      <c r="F27" s="1">
+        <v>53390.138276553102</v>
+      </c>
+      <c r="G27" s="2">
+        <v>826.81162324649301</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -724,8 +996,17 @@
       <c r="C28">
         <v>73.410290000000003</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>83.806545879602496</v>
+      </c>
+      <c r="F28" s="1">
+        <v>50581.2407948568</v>
+      </c>
+      <c r="G28" s="2">
+        <v>332.208649912331</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -735,8 +1016,17 @@
       <c r="C29">
         <v>49.283720000000002</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>111.39058524172999</v>
+      </c>
+      <c r="F29" s="1">
+        <v>67149.312977099195</v>
+      </c>
+      <c r="G29" s="2">
+        <v>266.05470737913402</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -746,8 +1036,17 @@
       <c r="C30">
         <v>30.47297</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>121.824324324324</v>
+      </c>
+      <c r="F30" s="1">
+        <v>73409.202702702707</v>
+      </c>
+      <c r="G30" s="2">
+        <v>1035.2432432432399</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -757,8 +1056,17 @@
       <c r="C31">
         <v>23.676259999999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>98.683453237410006</v>
+      </c>
+      <c r="F31" s="1">
+        <v>59501.820143884797</v>
+      </c>
+      <c r="G31" s="2">
+        <v>1105.41726618705</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -768,8 +1076,17 @@
       <c r="C32">
         <v>67.05</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>97.762500000000003</v>
+      </c>
+      <c r="F32" s="1">
+        <v>58986.262499999997</v>
+      </c>
+      <c r="G32" s="2">
+        <v>789.61249999999995</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -779,8 +1096,17 @@
       <c r="C33">
         <v>45.32</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>98.852000000000004</v>
+      </c>
+      <c r="F33" s="1">
+        <v>59604.536</v>
+      </c>
+      <c r="G33" s="2">
+        <v>337.62799999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -790,8 +1116,17 @@
       <c r="C34">
         <v>18.525929999999999</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>110.35849056603701</v>
+      </c>
+      <c r="F34" s="1">
+        <v>66514.471698113193</v>
+      </c>
+      <c r="G34" s="2">
+        <v>1623.4528301886701</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -801,8 +1136,17 @@
       <c r="C35">
         <v>1.0909089999999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>134.45454545454501</v>
+      </c>
+      <c r="F35" s="1">
+        <v>80985.818181818104</v>
+      </c>
+      <c r="G35" s="2">
+        <v>232.72727272727201</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -812,8 +1156,17 @@
       <c r="C36">
         <v>45.703780000000002</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>71.649159663865504</v>
+      </c>
+      <c r="F36" s="1">
+        <v>43286.1365546218</v>
+      </c>
+      <c r="G36" s="2">
+        <v>1053.0735294117601</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -823,8 +1176,17 @@
       <c r="C37">
         <v>87.723680000000002</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>84.988038277511905</v>
+      </c>
+      <c r="F37" s="1">
+        <v>51282.2440191387</v>
+      </c>
+      <c r="G37" s="2">
+        <v>835.79066985645898</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -834,8 +1196,17 @@
       <c r="C38">
         <v>48.5</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>127.375</v>
+      </c>
+      <c r="F38" s="1">
+        <v>76791</v>
+      </c>
+      <c r="G38" s="2">
+        <v>749.125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -845,8 +1216,17 @@
       <c r="C39">
         <v>40.839669999999998</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>98.084275436793405</v>
+      </c>
+      <c r="F39" s="1">
+        <v>59156.040082219901</v>
+      </c>
+      <c r="G39" s="2">
+        <v>499.96916752312399</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -856,8 +1236,17 @@
       <c r="C40">
         <v>36.721240000000002</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>94.907079646017607</v>
+      </c>
+      <c r="F40" s="1">
+        <v>57261.783185840701</v>
+      </c>
+      <c r="G40" s="2">
+        <v>213.59955752212301</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -867,8 +1256,17 @@
       <c r="C41">
         <v>53.2973</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>96.190990990990997</v>
+      </c>
+      <c r="F41" s="1">
+        <v>58013.358558558502</v>
+      </c>
+      <c r="G41" s="2">
+        <v>547.28468468468395</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -878,8 +1276,17 @@
       <c r="C42">
         <v>59.214010000000002</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <v>111.36575875486299</v>
+      </c>
+      <c r="F42" s="1">
+        <v>67128.603112840399</v>
+      </c>
+      <c r="G42" s="2">
+        <v>2035.50583657587</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -889,8 +1296,17 @@
       <c r="C43">
         <v>53.715739999999997</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <v>84.835025380710604</v>
+      </c>
+      <c r="F43" s="1">
+        <v>51191.147208121802</v>
+      </c>
+      <c r="G43" s="2">
+        <v>696.31725888324797</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -900,461 +1316,983 @@
       <c r="C44">
         <v>101.12690000000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <v>66.664450127877203</v>
+      </c>
+      <c r="F44" s="1">
+        <v>40292.014833759502</v>
+      </c>
+      <c r="G44" s="2">
+        <v>547.97442455242901</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45">
         <v>70.21875</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>66.6875</v>
+      </c>
+      <c r="F45" s="1">
+        <v>40321.9375</v>
+      </c>
+      <c r="G45" s="2">
+        <v>1026.03125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46">
         <v>78.958699999999993</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <v>89.687315634218294</v>
+      </c>
+      <c r="F46" s="1">
+        <v>54110.020648967497</v>
+      </c>
+      <c r="G46" s="2">
+        <v>535.23893805309694</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47">
         <v>11.06</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <v>75.12</v>
+      </c>
+      <c r="F47" s="1">
+        <v>45332.9</v>
+      </c>
+      <c r="G47" s="2">
+        <v>1278.3599999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48">
         <v>47.96895</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>46.007942238267098</v>
+      </c>
+      <c r="F48" s="1">
+        <v>27901.101805054099</v>
+      </c>
+      <c r="G48" s="2">
+        <v>367.32129963898899</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49">
         <v>63.229590000000002</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>89.132653061224403</v>
+      </c>
+      <c r="F49" s="1">
+        <v>53790.4387755102</v>
+      </c>
+      <c r="G49" s="2">
+        <v>143.93877551020401</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50">
         <v>29.402439999999999</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <v>67.121951219512198</v>
+      </c>
+      <c r="F50" s="1">
+        <v>40603.060975609696</v>
+      </c>
+      <c r="G50" s="2">
+        <v>699.13414634146295</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51">
         <v>398.5</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <v>36.5</v>
+      </c>
+      <c r="F51" s="1">
+        <v>22450.5</v>
+      </c>
+      <c r="G51" s="2">
+        <v>2567.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52">
         <v>37.138890000000004</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <v>97.1111111111111</v>
+      </c>
+      <c r="F52" s="1">
+        <v>58513.583333333299</v>
+      </c>
+      <c r="G52" s="2">
+        <v>309.194444444444</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53">
         <v>76.318119999999993</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E53">
+        <v>82.634899328859007</v>
+      </c>
+      <c r="F53" s="1">
+        <v>49885.790604026799</v>
+      </c>
+      <c r="G53" s="2">
+        <v>662.46711409395903</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54">
         <v>8.796875</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E54">
+        <v>126.71875</v>
+      </c>
+      <c r="F54" s="1">
+        <v>76351.859375</v>
+      </c>
+      <c r="G54" s="2">
+        <v>690.453125</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55">
         <v>53.257730000000002</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E55">
+        <v>94.4381443298969</v>
+      </c>
+      <c r="F55" s="1">
+        <v>56973.518041237097</v>
+      </c>
+      <c r="G55" s="2">
+        <v>737.11726804123703</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56">
         <v>65.508470000000003</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E56">
+        <v>101.38983050847401</v>
+      </c>
+      <c r="F56" s="1">
+        <v>61104.474576271103</v>
+      </c>
+      <c r="G56" s="2">
+        <v>2154.8474576271101</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57">
         <v>42.22222</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E57">
+        <v>72.6666666666666</v>
+      </c>
+      <c r="F57" s="1">
+        <v>43978.777777777701</v>
+      </c>
+      <c r="G57" s="2">
+        <v>1241.2222222222199</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58">
         <v>57.402679999999997</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E58">
+        <v>85.543624161073794</v>
+      </c>
+      <c r="F58" s="1">
+        <v>51633.3741610738</v>
+      </c>
+      <c r="G58" s="2">
+        <v>405.19295302013398</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59">
         <v>27.31054</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E59">
+        <v>86.678062678062602</v>
+      </c>
+      <c r="F59" s="1">
+        <v>52319.039886039798</v>
+      </c>
+      <c r="G59" s="2">
+        <v>878.13675213675197</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60">
         <v>51.251649999999998</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E60">
+        <v>96.934065934065899</v>
+      </c>
+      <c r="F60" s="1">
+        <v>58458.037362637297</v>
+      </c>
+      <c r="G60" s="2">
+        <v>201.67472527472501</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61">
         <v>46.847969999999997</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E61">
+        <v>102.35117773019201</v>
+      </c>
+      <c r="F61" s="1">
+        <v>61714.464668094202</v>
+      </c>
+      <c r="G61" s="2">
+        <v>2324.5674518201199</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62">
         <v>65.503820000000005</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E62">
+        <v>107.564885496183</v>
+      </c>
+      <c r="F62" s="1">
+        <v>64841.236641221301</v>
+      </c>
+      <c r="G62" s="2">
+        <v>713.22137404580099</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63">
         <v>80.118179999999995</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E63">
+        <v>44.545454545454497</v>
+      </c>
+      <c r="F63" s="1">
+        <v>27060.618181818099</v>
+      </c>
+      <c r="G63" s="2">
+        <v>182.89090909090899</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64">
         <v>71.578950000000006</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E64">
+        <v>127.578947368421</v>
+      </c>
+      <c r="F64" s="1">
+        <v>76868.105263157893</v>
+      </c>
+      <c r="G64" s="2">
+        <v>218.36842105263099</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65">
         <v>54.744759999999999</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <v>88.288461538461505</v>
+      </c>
+      <c r="F65" s="1">
+        <v>53247.382867132801</v>
+      </c>
+      <c r="G65" s="2">
+        <v>477.18531468531398</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66">
         <v>35.841349999999998</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E66">
+        <v>93.719551282051199</v>
+      </c>
+      <c r="F66" s="1">
+        <v>56534.801282051201</v>
+      </c>
+      <c r="G66" s="2">
+        <v>912.94070512820497</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67">
         <v>25.089169999999999</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E67">
+        <v>113.36305732484</v>
+      </c>
+      <c r="F67" s="1">
+        <v>68321.694267515893</v>
+      </c>
+      <c r="G67" s="2">
+        <v>1255.6815286624201</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68">
         <v>46.837040000000002</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E68">
+        <v>54.377777777777702</v>
+      </c>
+      <c r="F68" s="1">
+        <v>32926.037037037</v>
+      </c>
+      <c r="G68" s="2">
+        <v>634.62962962962899</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69">
         <v>67.98</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E69">
+        <v>23.84</v>
+      </c>
+      <c r="F69" s="1">
+        <v>14632.02</v>
+      </c>
+      <c r="G69" s="2">
+        <v>1052.92</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70">
         <v>134.9468</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E70">
+        <v>119.94680851063799</v>
+      </c>
+      <c r="F70" s="1">
+        <v>72261.765957446798</v>
+      </c>
+      <c r="G70" s="2">
+        <v>846.127659574468</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71">
         <v>31.31373</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E71">
+        <v>124.215686274509</v>
+      </c>
+      <c r="F71" s="1">
+        <v>74812.862745097998</v>
+      </c>
+      <c r="G71" s="2">
+        <v>393.13725490195998</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72">
         <v>131.6678</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E72">
+        <v>101.05704697986501</v>
+      </c>
+      <c r="F72" s="1">
+        <v>60959.050335570399</v>
+      </c>
+      <c r="G72" s="2">
+        <v>841.15100671140897</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73">
         <v>26.741520000000001</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E73">
+        <v>90.975767366720504</v>
+      </c>
+      <c r="F73" s="1">
+        <v>54888.250403877202</v>
+      </c>
+      <c r="G73" s="2">
+        <v>892.927302100161</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74">
         <v>89.208650000000006</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E74">
+        <v>100.363867684478</v>
+      </c>
+      <c r="F74" s="1">
+        <v>60527.048346055897</v>
+      </c>
+      <c r="G74" s="2">
+        <v>456.11959287531801</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75">
         <v>61.261189999999999</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E75">
+        <v>75.4402985074626</v>
+      </c>
+      <c r="F75" s="1">
+        <v>45566.195895522302</v>
+      </c>
+      <c r="G75" s="2">
+        <v>916.91231343283505</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76">
         <v>62.132530000000003</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E76">
+        <v>86.260240963855395</v>
+      </c>
+      <c r="F76" s="1">
+        <v>52051.996385542101</v>
+      </c>
+      <c r="G76" s="2">
+        <v>320.20843373493898</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77">
         <v>37.310339999999997</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E77">
+        <v>93.310344827586206</v>
+      </c>
+      <c r="F77" s="1">
+        <v>56252.758620689601</v>
+      </c>
+      <c r="G77" s="2">
+        <v>1617.6551724137901</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78">
         <v>47.629669999999997</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E78">
+        <v>78.2932242990654</v>
+      </c>
+      <c r="F78" s="1">
+        <v>47273.200934579399</v>
+      </c>
+      <c r="G78" s="2">
+        <v>353.19859813084099</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
       <c r="B79">
         <v>43.747999999999998</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E79">
+        <v>113.92</v>
+      </c>
+      <c r="F79" s="1">
+        <v>68657.528000000006</v>
+      </c>
+      <c r="G79" s="2">
+        <v>996.06</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
       <c r="B80">
         <v>65.799819999999997</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E80">
+        <v>85.547576301615806</v>
+      </c>
+      <c r="F80" s="1">
+        <v>51643.121184919197</v>
+      </c>
+      <c r="G80" s="2">
+        <v>368.18671454218997</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
       <c r="B81">
         <v>54.78754</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E81">
+        <v>92.118980169971607</v>
+      </c>
+      <c r="F81" s="1">
+        <v>55560.943342776198</v>
+      </c>
+      <c r="G81" s="2">
+        <v>801.94617563739303</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
       <c r="B82">
         <v>81.904309999999995</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E82">
+        <v>99.377990430622006</v>
+      </c>
+      <c r="F82" s="1">
+        <v>59931.023923444904</v>
+      </c>
+      <c r="G82" s="2">
+        <v>1546.54545454545</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83">
         <v>27.05</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E83">
+        <v>90.633333333333297</v>
+      </c>
+      <c r="F83" s="1">
+        <v>54690.216666666602</v>
+      </c>
+      <c r="G83" s="2">
+        <v>1098.81666666666</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
       <c r="B84">
         <v>60.272730000000003</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E84">
+        <v>106.515151515151</v>
+      </c>
+      <c r="F84" s="1">
+        <v>64205.505050505002</v>
+      </c>
+      <c r="G84" s="2">
+        <v>1620.55555555555</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
       <c r="B85">
         <v>51.22222</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E85">
+        <v>106.444444444444</v>
+      </c>
+      <c r="F85" s="1">
+        <v>64142.666666666599</v>
+      </c>
+      <c r="G85" s="2">
+        <v>1381.6111111111099</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
       <c r="B86">
         <v>108.47369999999999</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E86">
+        <v>110.210526315789</v>
+      </c>
+      <c r="F86" s="1">
+        <v>66507.052631578903</v>
+      </c>
+      <c r="G86" s="2">
+        <v>947.05263157894694</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
       <c r="B87">
         <v>66.897109999999998</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E87">
+        <v>102.646302250803</v>
+      </c>
+      <c r="F87" s="1">
+        <v>61893.093247588396</v>
+      </c>
+      <c r="G87" s="2">
+        <v>322.228295819935</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
       <c r="B88">
         <v>45.913040000000002</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E88">
+        <v>116.217391304347</v>
+      </c>
+      <c r="F88" s="1">
+        <v>70028.724637681094</v>
+      </c>
+      <c r="G88" s="2">
+        <v>571.65217391304304</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
       <c r="B89">
         <v>33.28866</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E89">
+        <v>88.989690721649396</v>
+      </c>
+      <c r="F89" s="1">
+        <v>53670.494845360801</v>
+      </c>
+      <c r="G89" s="2">
+        <v>4477.5051546391696</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
       <c r="B90">
         <v>41.142859999999999</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E90">
+        <v>95.993197278911495</v>
+      </c>
+      <c r="F90" s="1">
+        <v>57876.8843537414</v>
+      </c>
+      <c r="G90" s="2">
+        <v>519.44217687074797</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
       <c r="B91">
         <v>10.648149999999999</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E91">
+        <v>85.25</v>
+      </c>
+      <c r="F91" s="1">
+        <v>51438.680555555497</v>
+      </c>
+      <c r="G91" s="2">
+        <v>1160.3472222222199</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
       <c r="B92">
         <v>51.476379999999999</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E92">
+        <v>96.759842519684994</v>
+      </c>
+      <c r="F92" s="1">
+        <v>58368.216535432999</v>
+      </c>
+      <c r="G92" s="2">
+        <v>620.61811023621999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
       <c r="B93">
         <v>44.509799999999998</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E93">
+        <v>107.392156862745</v>
+      </c>
+      <c r="F93" s="1">
+        <v>64725.509803921501</v>
+      </c>
+      <c r="G93" s="2">
+        <v>2455.3725490195998</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
       <c r="B94">
         <v>261.5806</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E94">
+        <v>93.084710743801594</v>
+      </c>
+      <c r="F94" s="1">
+        <v>56141.037190082599</v>
+      </c>
+      <c r="G94" s="2">
+        <v>1121.64669421487</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
       <c r="B95">
         <v>89.636880000000005</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E95">
+        <v>94.281368821292702</v>
+      </c>
+      <c r="F95" s="1">
+        <v>56863.8479087452</v>
+      </c>
+      <c r="G95" s="2">
+        <v>542.73954372623496</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
       <c r="B96">
         <v>28.662579999999998</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E96">
+        <v>85.006134969325103</v>
+      </c>
+      <c r="F96" s="1">
+        <v>51301.0552147239</v>
+      </c>
+      <c r="G96" s="2">
+        <v>510.11042944785203</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
       <c r="B97">
         <v>77.60436</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E97">
+        <v>87.712729357798096</v>
+      </c>
+      <c r="F97" s="1">
+        <v>52939.191513761398</v>
+      </c>
+      <c r="G97" s="2">
+        <v>659.00974770642199</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
       <c r="B98">
         <v>64.422539999999998</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E98">
+        <v>113.760563380281</v>
+      </c>
+      <c r="F98" s="1">
+        <v>68527.838028169004</v>
+      </c>
+      <c r="G98" s="2">
+        <v>544.647887323943</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
       <c r="B99">
         <v>97.148939999999996</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E99">
+        <v>125.63829787234</v>
+      </c>
+      <c r="F99" s="1">
+        <v>75643.680851063793</v>
+      </c>
+      <c r="G99" s="2">
+        <v>1337.1914893617</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
       <c r="B100">
         <v>70.209299999999999</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E100">
+        <v>119.73255813953401</v>
+      </c>
+      <c r="F100" s="1">
+        <v>72084.546511627894</v>
+      </c>
+      <c r="G100" s="2">
+        <v>2342.0697674418602</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
       <c r="B101">
         <v>56.169490000000003</v>
+      </c>
+      <c r="E101">
+        <v>100.610169491525</v>
+      </c>
+      <c r="F101">
+        <v>60671.220338983003</v>
+      </c>
+      <c r="G101" s="2">
+        <v>1326.9830508474499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>